<commit_message>
Raise an error if encountering an unsupported input type
This check should be done earlier at the initial parsing of XLSForm
(during app launch), which is planned to be implemented shortly.
Example XLSForm has been updated to not raise this error.
</commit_message>
<xml_diff>
--- a/tests/data/stats4sd_example_xlsform_adapted.xlsx
+++ b/tests/data/stats4sd_example_xlsform_adapted.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC03D78-C1DA-194B-A3B6-C3F0E3DC3FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04BF33-DFA8-EB41-9F26-135A15F74D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="159">
   <si>
     <t>type</t>
   </si>
@@ -205,9 +205,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>geopoint</t>
-  </si>
-  <si>
     <t>begin group</t>
   </si>
   <si>
@@ -239,12 +236,6 @@
   </si>
   <si>
     <t>planned.holidays</t>
-  </si>
-  <si>
-    <t>survey_gps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.Please collect the GPS co-ordinate </t>
   </si>
   <si>
     <t xml:space="preserve">If the answer is none, please enter 0 </t>
@@ -1389,11 +1380,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1462,13 +1453,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.25">
@@ -1511,10 +1502,10 @@
     </row>
     <row r="5" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="11"/>
       <c r="H5" s="12"/>
@@ -1522,13 +1513,13 @@
     </row>
     <row r="6" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -1539,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="40" x14ac:dyDescent="0.25">
@@ -1550,279 +1541,277 @@
         <v>28</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="E9" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="F11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="K11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="13" t="s">
+    </row>
+    <row r="13" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="40" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="14" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="N14" s="18"/>
+    </row>
+    <row r="15" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="J16" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="N16" s="12"/>
+      <c r="O16" s="22"/>
+    </row>
+    <row r="17" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="23"/>
+    </row>
+    <row r="20" spans="1:15" ht="40" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="O11" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" s="13">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="F12" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="K12" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:17" ht="40" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="13" t="s">
+      <c r="I20" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="13" t="s">
+    </row>
+    <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="J17" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="22"/>
-    </row>
-    <row r="18" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="23"/>
-    </row>
-    <row r="21" spans="1:15" ht="40" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>98</v>
+      <c r="K21" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>93</v>
+        <v>152</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="C24" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="23"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I17">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>#REF! ="end repeat"</formula>
     </cfRule>
@@ -1892,35 +1881,35 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1930,133 +1919,133 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>58</v>
-      </c>
       <c r="C8" s="20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2066,58 +2055,58 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>83</v>
-      </c>
       <c r="D18" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>84</v>
-      </c>
       <c r="D19" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="C20" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>85</v>
-      </c>
       <c r="D20" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2127,145 +2116,145 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C31" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2321,7 +2310,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">CONCATENATE(YEAR(TODAY()),TEXT(MONTH(TODAY()),"00"),TEXT(DAY(TODAY()),"00"),TEXT(HOUR(NOW()),"00"),TEXT(MINUTE(NOW()),"00"))</f>
-        <v>202310222020</v>
+        <v>202311171537</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -2334,21 +2323,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000506DAE9941C6E48A9C55BDA8A72BDE7" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9b21557e877d51d9dc6baf46f65dd29b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e05110a1-bbe0-47e3-9ae9-9fd788bcb355" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4fa46b662fbc73e82b0d4dda846f7d25" ns3:_="">
     <xsd:import namespace="e05110a1-bbe0-47e3-9ae9-9fd788bcb355"/>
@@ -2512,24 +2486,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70EAE8BF-4C5E-4B5F-A4E0-A795DEA1A182}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC8168ED-4F79-43AE-B66F-F4A692FD5DE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2545,4 +2517,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70EAE8BF-4C5E-4B5F-A4E0-A795DEA1A182}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add population-blocked garbling to example XLSForm
</commit_message>
<xml_diff>
--- a/tests/data/stats4sd_example_xlsform_adapted.xlsx
+++ b/tests/data/stats4sd_example_xlsform_adapted.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04BF33-DFA8-EB41-9F26-135A15F74D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B51CEEA-B224-E343-AAAF-A96169FE550A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
   <si>
     <t>type</t>
   </si>
@@ -590,6 +590,15 @@
   </si>
   <si>
     <t>position(..)</t>
+  </si>
+  <si>
+    <t>like.travel</t>
+  </si>
+  <si>
+    <t>4.Do you enjoy travelling?</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -1380,11 +1389,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1567,15 +1576,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>42</v>
@@ -1584,186 +1593,195 @@
         <v>42</v>
       </c>
       <c r="P10" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="12" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="F11" s="10" t="s">
+      <c r="D12" s="11"/>
+      <c r="F12" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="K11" s="10" t="s">
+      <c r="H12" s="12"/>
+      <c r="K12" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:17" ht="40" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="13" t="s">
+    </row>
+    <row r="14" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+    <row r="15" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="D15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H16" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:15" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="J16" s="10" t="s">
+      <c r="D17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="J17" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="22"/>
-    </row>
-    <row r="17" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="N17" s="12"/>
+      <c r="O17" s="22"/>
+    </row>
+    <row r="18" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I18" s="24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="20" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="H19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="23"/>
-    </row>
-    <row r="20" spans="1:15" ht="40" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="D20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="21" spans="1:15" ht="40" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>42</v>
+        <v>151</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -1771,16 +1789,13 @@
         <v>103</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -1788,30 +1803,47 @@
         <v>103</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+    <row r="26" spans="1:15" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="H25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="23"/>
+      <c r="D26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="I18">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>#REF! ="end repeat"</formula>
     </cfRule>
@@ -2310,7 +2342,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">CONCATENATE(YEAR(TODAY()),TEXT(MONTH(TODAY()),"00"),TEXT(DAY(TODAY()),"00"),TEXT(HOUR(NOW()),"00"),TEXT(MINUTE(NOW()),"00"))</f>
-        <v>202311171537</v>
+        <v>202312081449</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -2323,6 +2355,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000506DAE9941C6E48A9C55BDA8A72BDE7" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9b21557e877d51d9dc6baf46f65dd29b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e05110a1-bbe0-47e3-9ae9-9fd788bcb355" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4fa46b662fbc73e82b0d4dda846f7d25" ns3:_="">
     <xsd:import namespace="e05110a1-bbe0-47e3-9ae9-9fd788bcb355"/>
@@ -2486,22 +2533,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70EAE8BF-4C5E-4B5F-A4E0-A795DEA1A182}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC8168ED-4F79-43AE-B66F-F4A692FD5DE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2517,21 +2566,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70EAE8BF-4C5E-4B5F-A4E0-A795DEA1A182}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>